<commit_message>
dodala mape, da bo bolj pregledno
</commit_message>
<xml_diff>
--- a/Zacetek.xlsx
+++ b/Zacetek.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\OPB\Mirjam-Spela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\FAX\3.letnik\OPB\Mirjam-Spela\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
-  <si>
-    <t>MONTH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -92,9 +89,6 @@
     <t>INT</t>
   </si>
   <si>
-    <t>ITEGER</t>
-  </si>
-  <si>
     <t>STRING</t>
   </si>
   <si>
@@ -114,6 +108,24 @@
   </si>
   <si>
     <t>BINARY</t>
+  </si>
+  <si>
+    <t>ŽRTVE</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>attack_id</t>
+  </si>
+  <si>
+    <t>SERIAL</t>
+  </si>
+  <si>
+    <t>ATTACK</t>
+  </si>
+  <si>
+    <t>country_name</t>
   </si>
 </sst>
 </file>
@@ -138,12 +150,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,9 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,15 +208,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -200,8 +226,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2457450" y="1114425"/>
-          <a:ext cx="1266825" cy="409575"/>
+          <a:off x="2476501" y="1476375"/>
+          <a:ext cx="1219199" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -276,16 +302,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -293,9 +319,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8572500" y="1085850"/>
-          <a:ext cx="1238250" cy="9525"/>
+        <a:xfrm flipV="1">
+          <a:off x="9458325" y="1466850"/>
+          <a:ext cx="1181100" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -323,16 +349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -340,13 +366,62 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4219575" y="762000"/>
-          <a:ext cx="5619750" cy="57151"/>
+        <a:xfrm>
+          <a:off x="4705350" y="1085850"/>
+          <a:ext cx="3514725" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 52033"/>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Elbow Connector 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="-1119189" y="1633537"/>
+          <a:ext cx="3076575" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 41950"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -636,186 +711,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q13"/>
+  <dimension ref="B2:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>25</v>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q8" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
+        <v>8</v>
       </c>
       <c r="P9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
       <c r="G12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>